<commit_message>
Updated Pathways Logic and Data
</commit_message>
<xml_diff>
--- a/Pathways Update/PathwaysRemove.xlsx
+++ b/Pathways Update/PathwaysRemove.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -31,15 +31,39 @@
     <t>Intake Date</t>
   </si>
   <si>
+    <t>Betty</t>
+  </si>
+  <si>
     <t>Pickle</t>
   </si>
   <si>
     <t>Crystal</t>
   </si>
   <si>
+    <t>Colby Jack Cheese</t>
+  </si>
+  <si>
+    <t>Sabre</t>
+  </si>
+  <si>
+    <t>Fleetwood</t>
+  </si>
+  <si>
+    <t>Mac</t>
+  </si>
+  <si>
+    <t>Bon Jovi</t>
+  </si>
+  <si>
     <t>Tigress</t>
   </si>
   <si>
+    <t>Breadstick</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
     <t>Maraschino</t>
   </si>
   <si>
@@ -64,15 +88,39 @@
     <t>Casher</t>
   </si>
   <si>
+    <t>57237345</t>
+  </si>
+  <si>
     <t>57091836</t>
   </si>
   <si>
     <t>57091845</t>
   </si>
   <si>
+    <t>57670293</t>
+  </si>
+  <si>
+    <t>57305889</t>
+  </si>
+  <si>
+    <t>57657154</t>
+  </si>
+  <si>
+    <t>57657157</t>
+  </si>
+  <si>
+    <t>57657185</t>
+  </si>
+  <si>
     <t>57657181</t>
   </si>
   <si>
+    <t>58011693</t>
+  </si>
+  <si>
+    <t>56455382</t>
+  </si>
+  <si>
     <t>57954349</t>
   </si>
   <si>
@@ -103,13 +151,28 @@
     <t>Dog</t>
   </si>
   <si>
+    <t>Bird</t>
+  </si>
+  <si>
+    <t>Cat Room G</t>
+  </si>
+  <si>
     <t>Feature Room 1</t>
   </si>
   <si>
+    <t>Dog A</t>
+  </si>
+  <si>
     <t>Foster Home</t>
   </si>
   <si>
-    <t>Dog A</t>
+    <t>Condo Rooms</t>
+  </si>
+  <si>
+    <t>Small Animals &amp; Exotics</t>
+  </si>
+  <si>
+    <t>Cat Room H</t>
   </si>
   <si>
     <t>Dog B</t>
@@ -118,10 +181,25 @@
     <t>Dog F</t>
   </si>
   <si>
+    <t>11/8/2024</t>
+  </si>
+  <si>
     <t>10/22/2024</t>
   </si>
   <si>
+    <t>1/17/2025</t>
+  </si>
+  <si>
+    <t>11/21/2024</t>
+  </si>
+  <si>
     <t>1/16/2025</t>
+  </si>
+  <si>
+    <t>3/13/2025</t>
+  </si>
+  <si>
+    <t>1/29/2025</t>
   </si>
   <si>
     <t>3/4/2025</t>
@@ -494,7 +572,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -522,16 +600,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -539,16 +617,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -556,16 +634,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -573,16 +651,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -590,16 +668,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -607,16 +685,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -624,16 +702,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -641,16 +719,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -658,16 +736,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -675,16 +753,16 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -692,16 +770,152 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
         <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for 8.12 and Pathways
</commit_message>
<xml_diff>
--- a/Pathways Update/PathwaysRemove.xlsx
+++ b/Pathways Update/PathwaysRemove.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdoptionsFosterMgr\Desktop\SPCAAutomation\Pathways Update\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5540D8F9-9776-41CB-B9E1-8CD4C77D9960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -29,13 +35,97 @@
   </si>
   <si>
     <t>Intake Date</t>
+  </si>
+  <si>
+    <t>Wishbone</t>
+  </si>
+  <si>
+    <t>Benji</t>
+  </si>
+  <si>
+    <t>Magnus</t>
+  </si>
+  <si>
+    <t>Scruffles</t>
+  </si>
+  <si>
+    <t>Huey</t>
+  </si>
+  <si>
+    <t>PUFF</t>
+  </si>
+  <si>
+    <t>57230680</t>
+  </si>
+  <si>
+    <t>58622374</t>
+  </si>
+  <si>
+    <t>58639325</t>
+  </si>
+  <si>
+    <t>58690617</t>
+  </si>
+  <si>
+    <t>58419285</t>
+  </si>
+  <si>
+    <t>58903460</t>
+  </si>
+  <si>
+    <t>58940639</t>
+  </si>
+  <si>
+    <t>Dog</t>
+  </si>
+  <si>
+    <t>Rabbit</t>
+  </si>
+  <si>
+    <t>Reptile/Amphibian</t>
+  </si>
+  <si>
+    <t>Dog E</t>
+  </si>
+  <si>
+    <t>Foster Home</t>
+  </si>
+  <si>
+    <t>Dog Adoptions A</t>
+  </si>
+  <si>
+    <t>If The Fur Fits</t>
+  </si>
+  <si>
+    <t>Dog Adoptions B</t>
+  </si>
+  <si>
+    <t>11/13/2024</t>
+  </si>
+  <si>
+    <t>6/2/2025</t>
+  </si>
+  <si>
+    <t>6/4/2025</t>
+  </si>
+  <si>
+    <t>6/19/2025</t>
+  </si>
+  <si>
+    <t>5/1/2025</t>
+  </si>
+  <si>
+    <t>7/17/25</t>
+  </si>
+  <si>
+    <t>7/19/25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,13 +188,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -142,7 +240,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -176,6 +274,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -210,9 +309,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -385,14 +485,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -407,6 +516,122 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>